<commit_message>
Made changes to template to correct small mistakes in spacing. Also addressed issue that crashed the code.
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
+++ b/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -50,6 +50,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="326">
   <si>
     <t xml:space="preserve">KPI Number</t>
   </si>
@@ -1238,52 +1239,19 @@
     <t xml:space="preserve">pass_value</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiene Copete y Cenefas-Comidas?</t>
-  </si>
-  <si>
     <t xml:space="preserve">POS option present</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiene las botellas necesarias por tamano-Comidas?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Minimum facings met</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Comidas? </t>
-  </si>
-  <si>
     <t xml:space="preserve">Mandatory SKUs found</t>
   </si>
   <si>
-    <t xml:space="preserve">La plataforma esta libre de objetos diferentes al portafolio valido-Comidas?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Coke purity</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiene Copete y Cenefas-Plat. Dinamicas 1?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 1? </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene las botellas necesarias por tamano-Plat. Dinamicas 1?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La plataforma esta libre de objetos diferentes al portafolio valido-Plat. Dinamicas 1?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene Copete y Cenefas-Plat. Dinamicas 2?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 2?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene las botellas necesarias por tamano-Plat. Dinamicas 2?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La plataforma esta libre de objetos diferentes al portafolio valido-Plat. Dinamicas 2?</t>
+    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 1?-Nacional</t>
   </si>
   <si>
     <t xml:space="preserve">Precios en cooler</t>
@@ -1377,9 +1345,6 @@
   </si>
   <si>
     <t xml:space="preserve">KPI Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Task/Template Group</t>
   </si>
   <si>
     <t xml:space="preserve">POS Option 1</t>
@@ -2169,10 +2134,10 @@
   </sheetPr>
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2180,12 +2145,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.1336032388664"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.3846153846154"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.3805668016194"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="116.117408906883"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5587044534413"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="117.186234817814"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -3168,7 +3133,7 @@
       </c>
       <c r="J38" s="10"/>
     </row>
-    <row r="39" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="32" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="2" t="n">
         <v>31</v>
       </c>
@@ -3578,7 +3543,7 @@
       <c r="I55" s="20"/>
       <c r="J55" s="10"/>
     </row>
-    <row r="56" customFormat="false" ht="32.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="2" t="n">
         <v>42</v>
       </c>
@@ -4066,7 +4031,7 @@
   <autoFilter ref="A1:J74">
     <filterColumn colId="3">
       <customFilters and="true">
-        <customFilter operator="equal" val="Llenado 75%-Nacional"/>
+        <customFilter operator="equal" val="Tiene las botellas necesarias por tamano-Comidas?-Nacional"/>
       </customFilters>
     </filterColumn>
   </autoFilter>
@@ -4098,11 +4063,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.7085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7125506072875"/>
@@ -4127,16 +4092,16 @@
         <v>6</v>
       </c>
       <c r="F1" s="80" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="G1" s="80" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="H1" s="80" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="I1" s="80" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="J1" s="80" t="s">
         <v>8</v>
@@ -4165,7 +4130,7 @@
         <v>144</v>
       </c>
       <c r="F2" s="81" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
@@ -4191,7 +4156,7 @@
         <v>144</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="G3" s="84"/>
       <c r="H3" s="81"/>
@@ -4217,7 +4182,7 @@
         <v>144</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="81"/>
@@ -4243,7 +4208,7 @@
         <v>144</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
@@ -4277,17 +4242,17 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="49.8097165991903"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="59.1295546558704"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="59.1295546558704"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="88.0526315789474"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="64.4858299595142"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="50.2388663967611"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="59.663967611336"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="85.3724696356275"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="59.663967611336"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="88.8016194331984"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="65.0202429149798"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="59" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="59" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="59" width="11.6761133603239"/>
@@ -4308,7 +4273,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -4373,7 +4338,7 @@
         <v>118</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>206</v>
@@ -4385,7 +4350,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="N2" s="85"/>
       <c r="O2" s="3" t="s">
@@ -4420,7 +4385,7 @@
         <v>124</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>206</v>
@@ -4432,7 +4397,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="N3" s="85"/>
       <c r="O3" s="3" t="s">
@@ -4467,10 +4432,10 @@
         <v>127</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="3" t="s">
@@ -4479,7 +4444,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="N4" s="85"/>
       <c r="O4" s="3" t="s">
@@ -4514,10 +4479,10 @@
         <v>131</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="3" t="s">
@@ -4526,7 +4491,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="N5" s="85"/>
       <c r="O5" s="3" t="s">
@@ -4561,10 +4526,10 @@
         <v>134</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="3" t="s">
@@ -4573,7 +4538,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="N6" s="85"/>
       <c r="O6" s="3" t="s">
@@ -4614,14 +4579,14 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.8137651821862"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="86.0161943319838"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="68.9838056680162"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="86.7651821862348"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.6275303643725"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6761133603239"/>
@@ -4642,22 +4607,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -4687,10 +4652,10 @@
         <v>13</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -4719,10 +4684,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -4750,10 +4715,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -4783,13 +4748,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="41" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I5" s="10" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="J5" s="10" t="n">
         <v>1</v>
@@ -4822,10 +4787,10 @@
         <v>13</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -4851,13 +4816,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="J7" s="10" t="n">
         <v>1</v>
@@ -4888,10 +4853,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -4917,10 +4882,10 @@
         <v>13</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -4946,10 +4911,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
       <c r="H10" s="81" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -4975,10 +4940,10 @@
         <v>13</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="H11" s="81" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -5002,10 +4967,10 @@
         <v>13</v>
       </c>
       <c r="G12" s="90" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
       <c r="H12" s="89" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="I12" s="89"/>
       <c r="J12" s="89"/>
@@ -5031,8 +4996,8 @@
   </sheetPr>
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5114,7 +5079,7 @@
         <v>186</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="I2" s="83"/>
       <c r="J2" s="84"/>
@@ -5125,7 +5090,7 @@
         <v>193</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="O2" s="82" t="s">
         <v>44</v>
@@ -5153,23 +5118,23 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.4210526315789"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7408906882591"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.2064777327935"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.4534412955466"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.7773279352227"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="51.417004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
@@ -5180,34 +5145,34 @@
         <v>5</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>6</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>325</v>
+        <v>195</v>
       </c>
       <c r="G1" s="34" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="H1" s="34" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="I1" s="34" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="J1" s="34" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="L1" s="34" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="M1" s="34" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="N1" s="34" t="s">
         <v>8</v>
@@ -5236,19 +5201,19 @@
         <v>206</v>
       </c>
       <c r="G2" s="91" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
       <c r="H2" s="91" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="I2" s="91" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="J2" s="20" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="K2" s="20" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>192</v>
@@ -5288,12 +5253,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.2024291497976"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="61.3805668016194"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="61.8056680161943"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="0" width="9.10526315789474"/>
@@ -5466,21 +5431,21 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="76.3765182186235"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.1295546558704"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="70.7004048582996"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.5991902834008"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="42.4210526315789"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.663967611336"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.5951417004049"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.2348178137652"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="42.7408906882591"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.9595141700405"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -5965,14 +5930,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.0283400809717"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.3481781376518"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.5627530364373"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -6102,11 +6067,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="23.8866396761134"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.9473684210526"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.5910931174089"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="158"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="159.392712550607"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -6360,21 +6325,21 @@
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.0971659919028"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="69.0931174089069"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="73.0566801619433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.5222672064777"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="69.7327935222672"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="73.6963562753036"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="59" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="93.4089068825911"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="94.2631578947368"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="59" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="59" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="13.3886639676113"/>
@@ -6873,27 +6838,27 @@
   </sheetPr>
   <dimension ref="A1:W3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="55.5951417004049"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.9514170040486"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="59.1295546558704"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="84.6234817813765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="62.9878542510121"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="45.9554655870445"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.3805668016194"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="59.663967611336"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="85.3724696356275"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="63.5222672064777"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -7107,19 +7072,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.0283400809717"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1376518218623"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="61.8056680161943"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.2429149797571"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -7309,17 +7274,17 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="59.7732793522267"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.3076923076923"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7340,7 +7305,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="54" t="n">
         <v>41</v>
       </c>
@@ -7348,16 +7313,16 @@
         <v>142</v>
       </c>
       <c r="C2" s="77" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>278</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>279</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="78" t="n">
         <v>42</v>
       </c>
@@ -7365,16 +7330,16 @@
         <v>142</v>
       </c>
       <c r="C3" s="77" t="s">
-        <v>280</v>
+        <v>151</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="n">
         <v>43</v>
       </c>
@@ -7382,16 +7347,16 @@
         <v>142</v>
       </c>
       <c r="C4" s="77" t="s">
-        <v>282</v>
+        <v>154</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="78" t="n">
         <v>44</v>
       </c>
@@ -7399,16 +7364,16 @@
         <v>142</v>
       </c>
       <c r="C5" s="36" t="s">
-        <v>284</v>
+        <v>157</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="78" t="n">
         <v>46</v>
       </c>
@@ -7416,16 +7381,16 @@
         <v>160</v>
       </c>
       <c r="C6" s="77" t="s">
-        <v>286</v>
+        <v>163</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="79" t="n">
         <v>47</v>
       </c>
@@ -7433,16 +7398,16 @@
         <v>160</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="78" t="n">
         <v>48</v>
       </c>
@@ -7450,16 +7415,16 @@
         <v>160</v>
       </c>
       <c r="C8" s="77" t="s">
-        <v>288</v>
+        <v>165</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="79" t="n">
         <v>49</v>
       </c>
@@ -7467,16 +7432,16 @@
         <v>160</v>
       </c>
       <c r="C9" s="36" t="s">
-        <v>289</v>
+        <v>166</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="78" t="n">
         <v>51</v>
       </c>
@@ -7484,16 +7449,16 @@
         <v>167</v>
       </c>
       <c r="C10" s="77" t="s">
-        <v>290</v>
+        <v>169</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="79" t="n">
         <v>52</v>
       </c>
@@ -7501,16 +7466,16 @@
         <v>167</v>
       </c>
       <c r="C11" s="77" t="s">
-        <v>291</v>
+        <v>170</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="78" t="n">
         <v>53</v>
       </c>
@@ -7518,16 +7483,16 @@
         <v>167</v>
       </c>
       <c r="C12" s="77" t="s">
-        <v>292</v>
+        <v>171</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="79" t="n">
         <v>54</v>
       </c>
@@ -7535,10 +7500,10 @@
         <v>167</v>
       </c>
       <c r="C13" s="77" t="s">
-        <v>293</v>
+        <v>172</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>1</v>
@@ -7552,10 +7517,10 @@
         <v>116</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Fixed spacing issues in the template
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
+++ b/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -51,6 +51,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="325">
   <si>
     <t xml:space="preserve">KPI Number</t>
   </si>
@@ -896,7 +897,7 @@
     <t xml:space="preserve">Tiene Copete y Cenefas-Plat. Dinamicas 1?-Nacional</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 1? -Nacional</t>
+    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 1?-Nacional</t>
   </si>
   <si>
     <t xml:space="preserve">Tiene las botellas necesarias por tamano-Plat. Dinamicas 1?-Nacional</t>
@@ -1249,9 +1250,6 @@
   </si>
   <si>
     <t xml:space="preserve">Coke purity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tiene los empaques mandatorios de portafolio-Plat. Dinamicas 1?-Nacional</t>
   </si>
   <si>
     <t xml:space="preserve">Precios en cooler</t>
@@ -2134,10 +2132,10 @@
   </sheetPr>
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="D63" activeCellId="0" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2145,12 +2143,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.5587044534413"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="61.8056680161943"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="117.186234817814"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.9878542510121"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="118.259109311741"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -3517,7 +3515,7 @@
       <c r="I54" s="20"/>
       <c r="J54" s="10"/>
     </row>
-    <row r="55" customFormat="false" ht="32.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2" t="n">
         <v>41</v>
       </c>
@@ -3569,7 +3567,7 @@
       <c r="I56" s="20"/>
       <c r="J56" s="10"/>
     </row>
-    <row r="57" customFormat="false" ht="32" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="2" t="n">
         <v>43</v>
       </c>
@@ -3595,7 +3593,7 @@
       <c r="I57" s="20"/>
       <c r="J57" s="10"/>
     </row>
-    <row r="58" customFormat="false" ht="32.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="2" t="n">
         <v>44</v>
       </c>
@@ -3669,7 +3667,7 @@
       <c r="I60" s="20"/>
       <c r="J60" s="10"/>
     </row>
-    <row r="61" customFormat="false" ht="75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="2" t="n">
         <v>46</v>
       </c>
@@ -3695,7 +3693,7 @@
       <c r="I61" s="20"/>
       <c r="J61" s="10"/>
     </row>
-    <row r="62" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="2" t="n">
         <v>47</v>
       </c>
@@ -3721,7 +3719,7 @@
       <c r="I62" s="20"/>
       <c r="J62" s="10"/>
     </row>
-    <row r="63" customFormat="false" ht="30" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="2" t="n">
         <v>48</v>
       </c>
@@ -3747,7 +3745,7 @@
       <c r="I63" s="20"/>
       <c r="J63" s="10"/>
     </row>
-    <row r="64" customFormat="false" ht="32" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="2" t="n">
         <v>49</v>
       </c>
@@ -3799,7 +3797,7 @@
       <c r="I65" s="20"/>
       <c r="J65" s="10"/>
     </row>
-    <row r="66" customFormat="false" ht="21.75" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="2" t="n">
         <v>51</v>
       </c>
@@ -3825,7 +3823,7 @@
       <c r="I66" s="20"/>
       <c r="J66" s="10"/>
     </row>
-    <row r="67" customFormat="false" ht="26.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="2" t="n">
         <v>52</v>
       </c>
@@ -3851,7 +3849,7 @@
       <c r="I67" s="20"/>
       <c r="J67" s="10"/>
     </row>
-    <row r="68" customFormat="false" ht="27" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="68" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="2" t="n">
         <v>53</v>
       </c>
@@ -3877,7 +3875,7 @@
       <c r="I68" s="20"/>
       <c r="J68" s="10"/>
     </row>
-    <row r="69" customFormat="false" ht="32.25" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="32.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="2" t="n">
         <v>54</v>
       </c>
@@ -4029,10 +4027,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:J74">
-    <filterColumn colId="3">
-      <customFilters and="true">
-        <customFilter operator="equal" val="Tiene las botellas necesarias por tamano-Comidas?-Nacional"/>
-      </customFilters>
+    <filterColumn colId="6">
+      <filters>
+        <filter val="Platformas"/>
+        <filter val="Platformas Scoring"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <mergeCells count="1">
@@ -4063,11 +4062,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.4210526315789"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.8178137651822"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.2064777327935"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7125506072875"/>
@@ -4092,16 +4091,16 @@
         <v>6</v>
       </c>
       <c r="F1" s="80" t="s">
+        <v>283</v>
+      </c>
+      <c r="G1" s="80" t="s">
         <v>284</v>
       </c>
-      <c r="G1" s="80" t="s">
+      <c r="H1" s="80" t="s">
         <v>285</v>
       </c>
-      <c r="H1" s="80" t="s">
+      <c r="I1" s="80" t="s">
         <v>286</v>
-      </c>
-      <c r="I1" s="80" t="s">
-        <v>287</v>
       </c>
       <c r="J1" s="80" t="s">
         <v>8</v>
@@ -4130,7 +4129,7 @@
         <v>144</v>
       </c>
       <c r="F2" s="81" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G2" s="81"/>
       <c r="H2" s="81"/>
@@ -4156,7 +4155,7 @@
         <v>144</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G3" s="84"/>
       <c r="H3" s="81"/>
@@ -4182,7 +4181,7 @@
         <v>144</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G4" s="84"/>
       <c r="H4" s="81"/>
@@ -4208,7 +4207,7 @@
         <v>144</v>
       </c>
       <c r="F5" s="82" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G5" s="82"/>
       <c r="H5" s="82"/>
@@ -4242,17 +4241,17 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="50.2388663967611"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="85.3724696356275"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="88.8016194331984"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="65.0202429149798"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="50.668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="89.5506072874494"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="65.5587044534413"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="59" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="59" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="59" width="11.6761133603239"/>
@@ -4273,7 +4272,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>5</v>
@@ -4338,7 +4337,7 @@
         <v>118</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>206</v>
@@ -4350,7 +4349,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N2" s="85"/>
       <c r="O2" s="3" t="s">
@@ -4385,7 +4384,7 @@
         <v>124</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H3" s="12" t="s">
         <v>206</v>
@@ -4397,7 +4396,7 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N3" s="85"/>
       <c r="O3" s="3" t="s">
@@ -4432,10 +4431,10 @@
         <v>127</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H4" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="3" t="s">
@@ -4444,7 +4443,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N4" s="85"/>
       <c r="O4" s="3" t="s">
@@ -4479,10 +4478,10 @@
         <v>131</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I5" s="12"/>
       <c r="J5" s="3" t="s">
@@ -4491,7 +4490,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N5" s="85"/>
       <c r="O5" s="3" t="s">
@@ -4526,10 +4525,10 @@
         <v>134</v>
       </c>
       <c r="G6" s="12" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="3" t="s">
@@ -4538,7 +4537,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N6" s="85"/>
       <c r="O6" s="3" t="s">
@@ -4579,14 +4578,14 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="34.8137651821862"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.0283400809717"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="86.7651821862348"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="69.6275303643725"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="87.5141700404858"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="70.2712550607288"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6761133603239"/>
@@ -4607,22 +4606,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>297</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>286</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>287</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -4652,10 +4651,10 @@
         <v>13</v>
       </c>
       <c r="G2" s="15" t="s">
+        <v>297</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>298</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>299</v>
       </c>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -4684,10 +4683,10 @@
         <v>13</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I3" s="11"/>
       <c r="J3" s="11"/>
@@ -4715,10 +4714,10 @@
         <v>13</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -4748,13 +4747,13 @@
         <v>13</v>
       </c>
       <c r="G5" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="I5" s="10" t="s">
         <v>302</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>303</v>
       </c>
       <c r="J5" s="10" t="n">
         <v>1</v>
@@ -4787,10 +4786,10 @@
         <v>13</v>
       </c>
       <c r="G6" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -4816,13 +4815,13 @@
         <v>13</v>
       </c>
       <c r="G7" s="41" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J7" s="10" t="n">
         <v>1</v>
@@ -4853,10 +4852,10 @@
         <v>13</v>
       </c>
       <c r="G8" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>306</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
@@ -4882,10 +4881,10 @@
         <v>13</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
@@ -4911,10 +4910,10 @@
         <v>13</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H10" s="81" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -4940,10 +4939,10 @@
         <v>13</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H11" s="81" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -4967,10 +4966,10 @@
         <v>13</v>
       </c>
       <c r="G12" s="90" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H12" s="89" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I12" s="89"/>
       <c r="J12" s="89"/>
@@ -5079,7 +5078,7 @@
         <v>186</v>
       </c>
       <c r="H2" s="83" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I2" s="83"/>
       <c r="J2" s="84"/>
@@ -5090,7 +5089,7 @@
         <v>193</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="O2" s="82" t="s">
         <v>44</v>
@@ -5124,13 +5123,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.7408906882591"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.0607287449393"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.668016194332"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="44.7773279352227"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="51.417004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.0971659919028"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="51.8461538461539"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -5145,7 +5144,7 @@
         <v>5</v>
       </c>
       <c r="D1" s="34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E1" s="34" t="s">
         <v>6</v>
@@ -5154,25 +5153,25 @@
         <v>195</v>
       </c>
       <c r="G1" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="H1" s="34" t="s">
         <v>314</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="I1" s="34" t="s">
         <v>315</v>
       </c>
-      <c r="I1" s="34" t="s">
+      <c r="J1" s="34" t="s">
         <v>316</v>
       </c>
-      <c r="J1" s="34" t="s">
+      <c r="K1" s="34" t="s">
         <v>317</v>
       </c>
-      <c r="K1" s="34" t="s">
+      <c r="L1" s="34" t="s">
         <v>318</v>
       </c>
-      <c r="L1" s="34" t="s">
+      <c r="M1" s="34" t="s">
         <v>319</v>
-      </c>
-      <c r="M1" s="34" t="s">
-        <v>320</v>
       </c>
       <c r="N1" s="34" t="s">
         <v>8</v>
@@ -5201,19 +5200,19 @@
         <v>206</v>
       </c>
       <c r="G2" s="91" t="s">
+        <v>320</v>
+      </c>
+      <c r="H2" s="91" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="91" t="s">
+      <c r="I2" s="91" t="s">
         <v>322</v>
       </c>
-      <c r="I2" s="91" t="s">
+      <c r="J2" s="20" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>324</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>325</v>
       </c>
       <c r="L2" s="20" t="s">
         <v>192</v>
@@ -5253,12 +5252,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.2024291497976"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.1740890688259"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.6315789473684"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="61.8056680161943"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="0" width="9.10526315789474"/>
@@ -5431,21 +5430,21 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="76.3765182186235"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="77.0202429149798"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.5951417004049"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.2348178137652"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="34.8137651821862"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="42.7408906882591"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="49.919028340081"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="71.8785425101215"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.0283400809717"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="43.17004048583"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.1740890688259"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -5930,14 +5929,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="35.8866396761134"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -6067,11 +6066,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="70.5910931174089"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="71.1255060728745"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="159.392712550607"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.8785425101215"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="160.890688259109"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -6332,14 +6331,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="56.4534412955466"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="69.7327935222672"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="56.8785425101215"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="70.3765182186235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="74.3400809716599"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="59" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="94.2631578947368"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="95.0161943319838"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="59" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="59" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="13.3886639676113"/>
@@ -6845,20 +6844,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.0242914979757"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.3805668016194"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.5627530364373"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="59.663967611336"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="85.3724696356275"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="63.5222672064777"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="46.3805668016194"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="56.4534412955466"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.8097165991903"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.8866396761134"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="60.2024291497976"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="86.1255060728745"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="64.0566801619433"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="46.7044534412956"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="32.7773279352227"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -7072,19 +7071,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.5263157894737"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.995951417004"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.3441295546559"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.2064777327935"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="62.8785425101215"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -7274,17 +7273,17 @@
   </sheetPr>
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.3076923076923"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="60.8421052631579"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.7773279352227"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7398,7 +7397,7 @@
         <v>160</v>
       </c>
       <c r="C7" s="77" t="s">
-        <v>282</v>
+        <v>164</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>279</v>
@@ -7517,7 +7516,7 @@
         <v>116</v>
       </c>
       <c r="C14" s="60" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
Fixed bug in extra spaces and updated price adherence
</commit_message>
<xml_diff>
--- a/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
+++ b/Projects/CCNAYARMX/Data/CCNayarTemplate_Nationalv0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -54,6 +54,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs!$A$1:$J$74</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1272,7 +1273,7 @@
     <t xml:space="preserve">Comidas</t>
   </si>
   <si>
-    <t xml:space="preserve">Ahorrack,Frutales,Nutricion</t>
+    <t xml:space="preserve">Ahorrack,Frutales,Nutricion,Hidratación</t>
   </si>
   <si>
     <t xml:space="preserve">Precios en Cooler</t>
@@ -2145,12 +2146,12 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.8461538461539"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.412955465587"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="120.400809716599"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="29.3522267206478"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="121.473684210526"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="11" style="0" width="10.7125506072875"/>
     <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.78542510121457"/>
@@ -4040,18 +4041,18 @@
   </sheetPr>
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.1376518218623"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.8502024291498"/>
     <col collapsed="false" hidden="false" max="9" min="7" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.7125506072875"/>
@@ -4149,7 +4150,7 @@
       <c r="K3" s="82"/>
       <c r="L3" s="82"/>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="81" t="n">
         <v>50</v>
       </c>
@@ -4226,17 +4227,17 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.5222672064777"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="61.2712550607287"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="61.2712550607287"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="91.1578947368421"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="66.6275303643725"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="59" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="51.9514170040486"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="59" width="61.7004048582996"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="59" width="88.4817813765182"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="61.7004048582996"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="59" width="91.9068825910931"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="59" width="67.2712550607288"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="14" min="13" style="59" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="59" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="59" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="59" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="59" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="59" width="11.6761133603239"/>
@@ -4563,14 +4564,14 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5627530364372"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.4574898785425"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="35.6720647773279"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="89.1214574898785"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.3400809716599"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="89.8744939271255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="71.9838056680162"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="11.6761133603239"/>
@@ -5108,13 +5109,13 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="40.7044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="41.0283400809717"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="45.9554655870445"/>
-    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="46.3805668016194"/>
+    <col collapsed="false" hidden="false" max="13" min="10" style="0" width="53.1295546558704"/>
     <col collapsed="false" hidden="false" max="1025" min="14" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -5237,12 +5238,12 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.4898785425101"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="49.8097165991903"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="63.412955465587"/>
-    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="6" style="0" width="63.9514170040486"/>
+    <col collapsed="false" hidden="false" max="13" min="11" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="11.3562753036437"/>
     <col collapsed="false" hidden="false" max="1023" min="16" style="0" width="9.10526315789474"/>
@@ -5415,21 +5416,21 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="78.3036437246964"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="79.0526315789474"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.2712550607287"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="50.7732793522267"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.1619433198381"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.2064777327935"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.4574898785425"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.7004048582996"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="51.2024291497976"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="73.6963562753036"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="33.5263157894737"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="35.6720647773279"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.2388663967611"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="9.10526315789474"/>
@@ -5914,14 +5915,14 @@
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.46153846153846"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.7449392712551"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="21.9595141700405"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.8866396761134"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="17" min="17" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="9.10526315789474"/>
@@ -6051,11 +6052,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="72.4129554655871"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.0566801619433"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="163.890688259109"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="165.392712550607"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.78542510121457"/>
   </cols>
@@ -6316,14 +6317,14 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="59" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="27.4210526315789"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="57.9514170040486"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="52.8097165991903"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="71.4493927125506"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="75.6275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="59" width="27.6356275303644"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="59" width="58.4858299595142"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="59" width="53.2388663967611"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="59" width="72.0890688259109"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="59" width="76.3765182186235"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="59" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="96.7287449392713"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="59" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="59" width="97.587044534413"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="59" width="8.67611336032389"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="59" width="8.46153846153846"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="59" width="13.3886639676113"/>
@@ -6829,20 +6830,20 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="57.417004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.5263157894737"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="61.2712550607287"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="87.6234817813765"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="65.2348178137652"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="47.3481781376518"/>
-    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="57.9514170040486"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="61.7004048582996"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="88.4817813765182"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="65.7692307692308"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="47.7732793522267"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="18" min="17" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="21" min="21" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="23" min="23" style="0" width="11.6761133603239"/>
@@ -7056,19 +7057,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4898785425101"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.995951417004"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.6356275303644"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.9514170040486"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.5910931174089"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="16" min="15" style="0" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="9.10526315789474"/>
   </cols>
@@ -7258,17 +7259,17 @@
   </sheetPr>
   <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="61.8056680161943"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="29.9919028340081"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="62.3441295546559"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.4210526315789"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>

</xml_diff>